<commit_message>
Small Update to Protokol
</commit_message>
<xml_diff>
--- a/Planing/Projekt_Protokoll.xlsx
+++ b/Planing/Projekt_Protokoll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HTL\3BHIF\SYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492936BF-6FB8-403D-92F6-C3FA5032E1C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFACBF24-89A8-4D43-ABCD-6AA8CB5F2B1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{0EB1387A-4401-440F-AEDA-2D1E6E2945D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0EB1387A-4401-440F-AEDA-2D1E6E2945D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Projet Overview" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +101,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,8 +129,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -130,20 +150,188 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -515,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C9F817-AD91-40BF-85AF-E2F9C315E132}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,49 +713,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="26"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="26"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="26"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="26"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="26"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="26"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="26"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="26"/>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="26"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -581,77 +769,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CED6F36-1EFC-47E2-8708-28110CD7A459}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="71.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>15.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="C4" s="13">
+        <v>44242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="C5" s="13">
+        <v>44256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="C6" s="13">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
-        <v>22.3</v>
+      <c r="C7" s="15">
+        <v>44277</v>
       </c>
     </row>
   </sheetData>
@@ -663,62 +858,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83CC64B-EC72-4F4D-A208-882C504C2D43}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
     <col min="2" max="2" width="162.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>